<commit_message>
Added basic reading and writing to Excel, non functional save button
</commit_message>
<xml_diff>
--- a/podatki.xlsx
+++ b/podatki.xlsx
@@ -1,25 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="10">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Cola</t>
+  </si>
+  <si>
+    <t>1L</t>
+  </si>
+  <si>
+    <t>5eur</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0eur</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -47,16 +83,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -73,10 +109,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -111,7 +147,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -146,7 +182,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -240,21 +276,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -271,7 +307,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -323,20 +359,131 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Got basic functionality all working. Input fields do not have special requirements, no deleting
</commit_message>
<xml_diff>
--- a/podatki.xlsx
+++ b/podatki.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -36,19 +36,40 @@
     <t>Cola</t>
   </si>
   <si>
-    <t>1L</t>
-  </si>
-  <si>
-    <t>5eur</t>
-  </si>
-  <si>
-    <t>Race</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>0eur</t>
+    <t>hmpf</t>
+  </si>
+  <si>
+    <t>esoihff</t>
+  </si>
+  <si>
+    <t>stood</t>
+  </si>
+  <si>
+    <t>dood</t>
+  </si>
+  <si>
+    <t>hood</t>
+  </si>
+  <si>
+    <t>asdfdsf</t>
+  </si>
+  <si>
+    <t>4444</t>
+  </si>
+  <si>
+    <t>afdhfdh</t>
+  </si>
+  <si>
+    <t>626226</t>
+  </si>
+  <si>
+    <t>2626</t>
+  </si>
+  <si>
+    <t>226fdh</t>
+  </si>
+  <si>
+    <t>Name555</t>
   </si>
 </sst>
 </file>
@@ -375,7 +396,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -419,13 +440,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -441,46 +462,46 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Basically finished. No deleting
</commit_message>
<xml_diff>
--- a/podatki.xlsx
+++ b/podatki.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
@@ -27,49 +27,13 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>8,9</t>
   </si>
   <si>
-    <t>test</t>
+    <t>8.8</t>
   </si>
   <si>
-    <t>Cola</t>
-  </si>
-  <si>
-    <t>hmpf</t>
-  </si>
-  <si>
-    <t>esoihff</t>
-  </si>
-  <si>
-    <t>stood</t>
-  </si>
-  <si>
-    <t>dood</t>
-  </si>
-  <si>
-    <t>hood</t>
-  </si>
-  <si>
-    <t>asdfdsf</t>
-  </si>
-  <si>
-    <t>4444</t>
-  </si>
-  <si>
-    <t>afdhfdh</t>
-  </si>
-  <si>
-    <t>626226</t>
-  </si>
-  <si>
-    <t>2626</t>
-  </si>
-  <si>
-    <t>226fdh</t>
-  </si>
-  <si>
-    <t>Name555</t>
+    <t>10.0</t>
   </si>
 </sst>
 </file>
@@ -388,26 +352,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A2:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -418,7 +371,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -429,13 +382,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -446,62 +399,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>